<commit_message>
Revised excel creation , code refactoring
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\Workplace\AutoNewFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\Workplace\AutoNewProfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Template" sheetId="5" r:id="rId1"/>
-    <sheet name="AutoData-Template" sheetId="4" r:id="rId2"/>
+    <sheet name="AutoData-Template" sheetId="8" r:id="rId2"/>
     <sheet name="8H-Template" sheetId="2" r:id="rId3"/>
     <sheet name="12H-Template" sheetId="7" r:id="rId4"/>
     <sheet name="Final8H-Template" sheetId="1" r:id="rId5"/>
@@ -959,7 +959,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1186,50 +1186,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="2" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1241,6 +1197,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="2" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1259,47 +1259,35 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1914,15 +1902,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -1981,9 +1969,9 @@
       <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -2047,40 +2035,40 @@
       <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="103" t="s">
+      <c r="D9" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="103" t="s">
+      <c r="E9" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="103" t="s">
+      <c r="F9" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="103" t="s">
+      <c r="G9" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="103" t="s">
+      <c r="H9" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="103" t="s">
+      <c r="I9" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="103" t="s">
+      <c r="J9" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="103" t="s">
+      <c r="K9" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="103" t="s">
+      <c r="L9" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="103" t="s">
+      <c r="M9" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="N9" s="103" t="s">
+      <c r="N9" s="87" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2088,40 +2076,40 @@
       <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="104" t="s">
+      <c r="F10" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="104" t="s">
+      <c r="G10" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="104" t="s">
+      <c r="I10" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="105" t="s">
+      <c r="J10" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="103" t="s">
+      <c r="K10" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="103" t="s">
+      <c r="L10" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="103" t="s">
+      <c r="M10" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="103" t="s">
+      <c r="N10" s="87" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2129,40 +2117,40 @@
       <c r="B11" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="103" t="s">
+      <c r="E11" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="106" t="s">
+      <c r="F11" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="104" t="s">
+      <c r="G11" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="104" t="s">
+      <c r="H11" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="104" t="s">
+      <c r="I11" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="104" t="s">
+      <c r="J11" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="104" t="s">
+      <c r="M11" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="N11" s="105" t="s">
+      <c r="N11" s="89" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2184,211 +2172,209 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="101" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="100" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="100" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="8.88671875" style="100" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="100" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="100" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="17"/>
+    <col min="1" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="1" customWidth="1"/>
+    <col min="7" max="14" width="8.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="88"/>
-      <c r="J1" s="89" t="s">
+      <c r="I1" s="99"/>
+      <c r="J1" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89" t="s">
+      <c r="N1" s="99"/>
+      <c r="O1" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="89" t="s">
+      <c r="P1" s="100" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
     </row>
     <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="93"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
     </row>
     <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="95"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-    </row>
-    <row r="5" spans="1:16" s="98" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="92"/>
-    </row>
-    <row r="6" spans="1:16" s="98" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="92"/>
-    </row>
-    <row r="7" spans="1:16" s="98" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="92"/>
-    </row>
-    <row r="8" spans="1:16" s="98" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-    </row>
-    <row r="9" spans="1:16" s="98" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="92"/>
-      <c r="O9" s="92"/>
-      <c r="P9" s="92"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+    </row>
+    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="101"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+    </row>
+    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="103"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+    </row>
+    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="103"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+    </row>
+    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="103"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="103"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="103"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2399,19 +2385,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="108"/>
+    <col min="1" max="1" width="8.88671875" style="92"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="7.77734375" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
     <col min="8" max="10" width="8.109375" customWidth="1"/>
     <col min="11" max="11" width="14.21875" customWidth="1"/>
     <col min="12" max="12" width="14.21875" style="20" customWidth="1"/>
@@ -2457,7 +2443,7 @@
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:25" s="73" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="91" t="s">
         <v>91</v>
       </c>
       <c r="B5" s="80" t="s">
@@ -2524,7 +2510,7 @@
       <c r="Y5" s="74"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="127"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="72"/>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
@@ -2572,7 +2558,7 @@
       <c r="V6" s="32"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="127"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="59"/>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -2620,7 +2606,7 @@
       <c r="V7" s="32"/>
     </row>
     <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="127"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="59"/>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
@@ -2668,7 +2654,7 @@
       <c r="V8" s="32"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="127"/>
+      <c r="A9" s="95"/>
       <c r="B9" s="59"/>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
@@ -2716,7 +2702,7 @@
       <c r="V9" s="32"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="127"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="59"/>
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
@@ -2764,7 +2750,7 @@
       <c r="V10" s="32"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="127"/>
+      <c r="A11" s="95"/>
       <c r="B11" s="57"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
@@ -2812,7 +2798,7 @@
       <c r="V11" s="32"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
+      <c r="A12" s="95"/>
       <c r="B12" s="57"/>
       <c r="C12" s="56"/>
       <c r="D12" s="56"/>
@@ -2860,7 +2846,7 @@
       <c r="V12" s="32"/>
     </row>
     <row r="13" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="128"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="44"/>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
@@ -3050,19 +3036,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="125"/>
+    <col min="1" max="1" width="8.88671875" style="93"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="7.77734375" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
     <col min="8" max="10" width="8.109375" customWidth="1"/>
     <col min="11" max="11" width="14.21875" customWidth="1"/>
     <col min="12" max="12" width="14.21875" style="20" customWidth="1"/>
@@ -3108,7 +3094,7 @@
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:25" s="73" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="94" t="s">
         <v>91</v>
       </c>
       <c r="B5" s="80" t="s">
@@ -3175,7 +3161,7 @@
       <c r="Y5" s="74"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="127"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="72"/>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
@@ -3223,7 +3209,7 @@
       <c r="V6" s="32"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="127"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="59"/>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -3271,7 +3257,7 @@
       <c r="V7" s="32"/>
     </row>
     <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="127"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="59"/>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
@@ -3319,7 +3305,7 @@
       <c r="V8" s="32"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="127"/>
+      <c r="A9" s="95"/>
       <c r="B9" s="59"/>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
@@ -3367,7 +3353,7 @@
       <c r="V9" s="32"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="127"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="59"/>
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
@@ -3415,7 +3401,7 @@
       <c r="V10" s="32"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="127"/>
+      <c r="A11" s="95"/>
       <c r="B11" s="57"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
@@ -3463,7 +3449,7 @@
       <c r="V11" s="32"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
+      <c r="A12" s="95"/>
       <c r="B12" s="57"/>
       <c r="C12" s="56"/>
       <c r="D12" s="56"/>
@@ -3505,7 +3491,7 @@
       <c r="V12" s="32"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="127"/>
+      <c r="A13" s="95"/>
       <c r="B13" s="57"/>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
@@ -3547,7 +3533,7 @@
       <c r="V13" s="32"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="127"/>
+      <c r="A14" s="95"/>
       <c r="B14" s="57"/>
       <c r="C14" s="56"/>
       <c r="D14" s="56"/>
@@ -3589,7 +3575,7 @@
       <c r="V14" s="32"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="127"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="57"/>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
@@ -3631,7 +3617,7 @@
       <c r="V15" s="32"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="127"/>
+      <c r="A16" s="95"/>
       <c r="B16" s="57"/>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
@@ -3679,7 +3665,7 @@
       <c r="V16" s="32"/>
     </row>
     <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="128"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="44"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
@@ -3746,7 +3732,7 @@
       <c r="R20" s="28"/>
     </row>
     <row r="21" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="125"/>
+      <c r="A21" s="93"/>
       <c r="B21" s="27" t="s">
         <v>17</v>
       </c>
@@ -3770,7 +3756,7 @@
       <c r="Q21" s="18"/>
     </row>
     <row r="22" spans="1:22" s="19" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="125"/>
+      <c r="A22" s="93"/>
       <c r="B22" s="24" t="str">
         <f>IF(G17&gt;1,G17,"")</f>
         <v/>
@@ -3797,7 +3783,7 @@
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="125"/>
+      <c r="A23" s="93"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
@@ -3815,7 +3801,7 @@
       <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="125"/>
+      <c r="A24" s="93"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
@@ -3896,14 +3882,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3912,12 +3898,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="118"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -3944,10 +3930,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4041,11 +4027,11 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="3:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
@@ -4059,17 +4045,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="C2:H3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
@@ -4104,14 +4090,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4120,12 +4106,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="118"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4152,10 +4138,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4293,11 +4279,11 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="3:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
       <c r="F17" s="9"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
@@ -4311,12 +4297,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I15:J15"/>
@@ -4326,6 +4306,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed calculated productity formula
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\Workplace\AutoNewProfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\WebfactoryDataCollection-dev-3.9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1259,6 +1259,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1279,9 +1282,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3037,7 +3037,7 @@
   <dimension ref="A2:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3235,7 +3235,7 @@
         <v/>
       </c>
       <c r="N7" s="48" t="str">
-        <f t="shared" ref="N7:N17" si="4">IFERROR(IF(G7&gt;1,(G7/(D7*1)),""),"")</f>
+        <f>IFERROR(IF(G7&gt;1,(G7/(D7*2)),""),"")</f>
         <v/>
       </c>
       <c r="O7" s="48" t="str">
@@ -3283,7 +3283,7 @@
         <v/>
       </c>
       <c r="N8" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G8&gt;1,(G8/(D8*3)),""),"")</f>
         <v/>
       </c>
       <c r="O8" s="48" t="str">
@@ -3331,7 +3331,7 @@
         <v/>
       </c>
       <c r="N9" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G9&gt;1,(G9/(D9*4)),""),"")</f>
         <v/>
       </c>
       <c r="O9" s="48" t="str">
@@ -3379,7 +3379,7 @@
         <v/>
       </c>
       <c r="N10" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G10&gt;1,(G10/(D10*5)),""),"")</f>
         <v/>
       </c>
       <c r="O10" s="48" t="str">
@@ -3427,7 +3427,7 @@
         <v/>
       </c>
       <c r="N11" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G11&gt;1,(G11/(D11*6)),""),"")</f>
         <v/>
       </c>
       <c r="O11" s="48" t="str">
@@ -3475,7 +3475,7 @@
         <v/>
       </c>
       <c r="N12" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G12&gt;1,(G12/(D12*7)),""),"")</f>
         <v/>
       </c>
       <c r="O12" s="48" t="str">
@@ -3517,7 +3517,7 @@
         <v/>
       </c>
       <c r="N13" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G13&gt;1,(G13/(D13*8)),""),"")</f>
         <v/>
       </c>
       <c r="O13" s="48" t="str">
@@ -3559,7 +3559,7 @@
         <v/>
       </c>
       <c r="N14" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G14&gt;1,(G14/(D14*9)),""),"")</f>
         <v/>
       </c>
       <c r="O14" s="48" t="str">
@@ -3601,7 +3601,7 @@
         <v/>
       </c>
       <c r="N15" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G15&gt;1,(G15/(D15*10)),""),"")</f>
         <v/>
       </c>
       <c r="O15" s="48" t="str">
@@ -3643,7 +3643,7 @@
         <v/>
       </c>
       <c r="N16" s="48" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G16&gt;1,(G16/(D16*11)),""),"")</f>
         <v/>
       </c>
       <c r="O16" s="48" t="str">
@@ -3691,7 +3691,7 @@
         <v/>
       </c>
       <c r="N17" s="36" t="str">
-        <f t="shared" si="4"/>
+        <f>IFERROR(IF(G17&gt;1,(G17/(D17*12)),""),"")</f>
         <v/>
       </c>
       <c r="O17" s="36" t="str">
@@ -3882,14 +3882,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3898,12 +3898,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="117"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="119"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="120"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -3930,10 +3930,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="120" t="s">
+      <c r="I4" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="121"/>
+      <c r="J4" s="122"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4027,11 +4027,11 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="3:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="122"/>
-      <c r="E13" s="122"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
@@ -4045,17 +4045,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:E13"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="C2:H3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
@@ -4090,14 +4090,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4106,12 +4106,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="117"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="119"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="120"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4138,10 +4138,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="120" t="s">
+      <c r="I4" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="121"/>
+      <c r="J4" s="122"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4279,11 +4279,11 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="3:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
       <c r="F17" s="9"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
@@ -4297,6 +4297,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I15:J15"/>
@@ -4306,12 +4312,6 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed data structure in Template
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\WebfactoryDataCollection-dev-3.9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intel\456\ProjectNewV2\WebfactoryDataCollection-dev-6.9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Template" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
   <si>
     <t>Hodinový výkon - sledovanie</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Stĺpec9</t>
   </si>
   <si>
-    <t>8H-Ranná</t>
-  </si>
-  <si>
     <t>6:00-7:00</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
     <t>13:00-14:00</t>
   </si>
   <si>
-    <t>8H-Poobedná</t>
-  </si>
-  <si>
     <t>14:00-15:00</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>21:00-22:00</t>
   </si>
   <si>
-    <t>8H-Nočná</t>
-  </si>
-  <si>
     <t>22:00-23:00</t>
   </si>
   <si>
@@ -299,16 +290,19 @@
     <t>Stĺpec13</t>
   </si>
   <si>
-    <t>12H-Ranná</t>
-  </si>
-  <si>
-    <t>12H-Nočná</t>
-  </si>
-  <si>
     <t>ShiftCheck</t>
   </si>
   <si>
     <t>cas ziskania data</t>
+  </si>
+  <si>
+    <t>Ranná</t>
+  </si>
+  <si>
+    <t>Nočná</t>
+  </si>
+  <si>
+    <t>Poobedná</t>
   </si>
 </sst>
 </file>
@@ -1259,29 +1253,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1891,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1943,31 +1937,31 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>62</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" t="s">
-        <v>64</v>
       </c>
       <c r="L4" s="86"/>
       <c r="M4" s="86"/>
@@ -1975,65 +1969,65 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>67</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>69</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>70</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>71</v>
-      </c>
-      <c r="I5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>76</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>77</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>78</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>79</v>
-      </c>
-      <c r="H6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C9" s="87" t="s">
         <v>48</v>
@@ -2060,102 +2054,101 @@
         <v>55</v>
       </c>
       <c r="K9" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="87" t="s">
         <v>84</v>
-      </c>
-      <c r="L9" s="87" t="s">
-        <v>85</v>
-      </c>
-      <c r="M9" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="87" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="E10" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="88" t="s">
+      <c r="F10" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="88" t="s">
+      <c r="G10" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="88" t="s">
+      <c r="H10" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="88" t="s">
+      <c r="I10" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="88" t="s">
+      <c r="J10" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="89" t="s">
+      <c r="K10" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="87" t="s">
+      <c r="L10" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="87" t="s">
+      <c r="N10" s="87" t="s">
         <v>67</v>
-      </c>
-      <c r="M10" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="N10" s="87" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="F11" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="87" t="s">
+      <c r="G11" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="90" t="s">
+      <c r="H11" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="I11" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="88" t="s">
+      <c r="K11" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="88" t="s">
+      <c r="L11" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="88" t="s">
+      <c r="M11" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="88" t="s">
+      <c r="N11" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="88" t="s">
-        <v>80</v>
-      </c>
-      <c r="M11" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" s="89" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vqzIoE7vuPpjff7xj3DmHN2UhQX9HUo7O8ok1gtkE4LQ/8rq2YZhm0p98e5oFw9jCKMoEDY5alDn/6qZiopQxg==" saltValue="lXEw6qDY+WvXM8uICCiSsw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="2">
@@ -2226,7 +2219,7 @@
       </c>
       <c r="N1" s="99"/>
       <c r="O1" s="100" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="P1" s="100" t="s">
         <v>35</v>
@@ -2444,7 +2437,7 @@
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:25" s="73" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="91" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B5" s="80" t="s">
         <v>32</v>
@@ -3036,7 +3029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -3095,7 +3088,7 @@
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:25" s="73" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="94" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B5" s="80" t="s">
         <v>32</v>
@@ -3882,14 +3875,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3898,12 +3891,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="118"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -3930,10 +3923,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4027,11 +4020,11 @@
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="3:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
@@ -4045,17 +4038,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="C2:H3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
@@ -4090,14 +4083,14 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4106,12 +4099,12 @@
       </c>
     </row>
     <row r="3" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="118"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4138,10 +4131,10 @@
       <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4279,11 +4272,11 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="3:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
       <c r="F17" s="9"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
@@ -4297,12 +4290,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I15:J15"/>
@@ -4312,6 +4299,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>

</xml_diff>